<commit_message>
Auto open test report implemented
</commit_message>
<xml_diff>
--- a/STAF/packages/data.xlsx
+++ b/STAF/packages/data.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Step 1</t>
   </si>
@@ -39,23 +39,35 @@
     <t>Step 6</t>
   </si>
   <si>
-    <t>Step 7</t>
-  </si>
-  <si>
-    <t>Step 8</t>
-  </si>
-  <si>
-    <t>Step 9</t>
-  </si>
-  <si>
-    <t>Do something</t>
+    <t>Step Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Enter valid user name.</t>
+  </si>
+  <si>
+    <t>Navigate to URL.</t>
+  </si>
+  <si>
+    <t>Enter valid password.</t>
+  </si>
+  <si>
+    <t>Click Login button.</t>
+  </si>
+  <si>
+    <t>Verify user navigated to Home Page.</t>
+  </si>
+  <si>
+    <t>Click SignOut button.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +75,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -84,8 +117,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,90 +408,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel Reader added to test.
</commit_message>
<xml_diff>
--- a/STAF/packages/data.xlsx
+++ b/STAF/packages/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Step 1</t>
   </si>
@@ -61,13 +61,28 @@
   </si>
   <si>
     <t>Click SignOut button.</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Botton not visable!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +101,22 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -127,6 +158,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -411,13 +451,15 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -427,8 +469,12 @@
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -444,6 +490,9 @@
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="C2" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -452,6 +501,9 @@
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="C3" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -460,6 +512,9 @@
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="C4" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -468,6 +523,12 @@
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -476,6 +537,9 @@
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="C6" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -483,6 +547,9 @@
       </c>
       <c r="B7" s="3" t="s">
         <v>13</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>